<commit_message>
Updating Benchmarks with RDD Ref Part 1
</commit_message>
<xml_diff>
--- a/Benchmarks.xlsx
+++ b/Benchmarks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\msft-linalg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB9A6A28-E393-4CDA-8F87-72A88E0215DC}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47BC2D2-6FA7-49C4-9F35-E61F4095B5AF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34560" windowHeight="14976" xr2:uid="{36E862E2-4E59-4E4D-AB5D-4617D30FDC5B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25896" windowHeight="10104" xr2:uid="{36E862E2-4E59-4E4D-AB5D-4617D30FDC5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Benchmarks" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Result size</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>10000x10000*10000x10000</t>
+  </si>
+  <si>
+    <t>GPU 1 Node(12 Core)</t>
+  </si>
+  <si>
+    <t>CPU 1 Node(16 Core)</t>
+  </si>
+  <si>
+    <t>Sparseness</t>
+  </si>
+  <si>
+    <t>GPU 12 Node (+Head)</t>
+  </si>
+  <si>
+    <t>CPU 12 Node(16 Core)</t>
+  </si>
+  <si>
+    <t>REF(RDD) 1 GPU</t>
   </si>
 </sst>
 </file>
@@ -428,144 +446,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F45AFE7-866D-4F2A-AFF3-7E9866C2F309}">
-  <dimension ref="A2:B17"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.77734375" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="4" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>535</v>
+      </c>
+      <c r="E3">
+        <v>1745</v>
+      </c>
+      <c r="G3">
+        <v>4809</v>
+      </c>
+      <c r="H3">
+        <v>4972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>248</v>
+      </c>
+      <c r="E4">
+        <v>1003</v>
+      </c>
+      <c r="G4">
+        <v>2414</v>
+      </c>
+      <c r="H4">
+        <v>2420</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>100</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>216</v>
+      </c>
+      <c r="E5">
+        <v>42042</v>
+      </c>
+      <c r="G5">
+        <v>2213</v>
+      </c>
+      <c r="H5">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>301</v>
+      </c>
+      <c r="E6">
+        <v>41615</v>
+      </c>
+      <c r="G6">
+        <v>2330</v>
+      </c>
+      <c r="H6">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1000</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>318</v>
+      </c>
+      <c r="E7">
+        <v>44620</v>
+      </c>
+      <c r="G7">
+        <v>2276</v>
+      </c>
+      <c r="H7">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10000</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>0.1</v>
+      </c>
+      <c r="D8">
+        <v>373</v>
+      </c>
+      <c r="E8">
+        <v>45099</v>
+      </c>
+      <c r="G8">
+        <v>2952</v>
+      </c>
+      <c r="H8">
+        <v>2694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1000</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>6396</v>
+      </c>
+      <c r="E9">
+        <v>101450</v>
+      </c>
+      <c r="G9">
+        <v>3634</v>
+      </c>
+      <c r="H9">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10000</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+      <c r="D10">
+        <v>6631</v>
+      </c>
+      <c r="E10">
+        <v>107202</v>
+      </c>
+      <c r="G10">
+        <v>6958</v>
+      </c>
+      <c r="H10">
+        <v>6866</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>100000</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="D11">
+        <v>7470</v>
+      </c>
+      <c r="E11">
+        <v>110310</v>
+      </c>
+      <c r="G11">
+        <v>37418</v>
+      </c>
+      <c r="H11">
+        <v>38125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1000000</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>0.01</v>
+      </c>
+      <c r="D12">
+        <v>17014</v>
+      </c>
+      <c r="E12">
+        <v>177254</v>
+      </c>
+      <c r="G12">
+        <v>654384</v>
+      </c>
+      <c r="H12">
+        <v>645526</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>10000</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>6617119</v>
+      </c>
+      <c r="G13">
+        <v>97630</v>
+      </c>
+      <c r="H13">
+        <v>15388</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>100000</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+      <c r="E14">
+        <v>6651854</v>
+      </c>
+      <c r="G14">
+        <v>398520</v>
+      </c>
+      <c r="H14">
+        <v>708049</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1000000</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>0.01</v>
+      </c>
+      <c r="E15">
+        <v>6772861</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10000000</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>1E-4</v>
+      </c>
+      <c r="E16">
+        <v>10812616</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>100000000</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
+      </c>
+      <c r="C17">
+        <v>1E-4</v>
+      </c>
+      <c r="E17">
+        <v>47242268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>